<commit_message>
Выбор threshhold for NA/0 - 95%. Перезапись final_data
</commit_message>
<xml_diff>
--- a/data/originals/percentage_by_patient.xlsx
+++ b/data/originals/percentage_by_patient.xlsx
@@ -359,3050 +359,3050 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>369</v>
       </c>
       <c r="B2" t="n">
-        <v>18.0764774044032</v>
+        <v>93.38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>278</v>
       </c>
       <c r="B3" t="n">
-        <v>14.4843568945539</v>
+        <v>85.14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="B4" t="n">
-        <v>18.1923522595597</v>
+        <v>84.27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>325</v>
       </c>
       <c r="B5" t="n">
-        <v>20.973348783314</v>
+        <v>83.84</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>208</v>
       </c>
       <c r="B6" t="n">
-        <v>17.2653534183082</v>
+        <v>82.86</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="B7" t="n">
-        <v>20.6257242178447</v>
+        <v>82.75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="B8" t="n">
-        <v>20.3939745075319</v>
+        <v>82.65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>268</v>
       </c>
       <c r="B9" t="n">
-        <v>18.8489764387795</v>
+        <v>82.65</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>267</v>
       </c>
       <c r="B10" t="n">
-        <v>15.7976052529934</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="B11" t="n">
-        <v>18.5786017767478</v>
+        <v>80.91</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>377</v>
       </c>
       <c r="B12" t="n">
-        <v>16.0293549633063</v>
+        <v>80.8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>363</v>
       </c>
       <c r="B13" t="n">
-        <v>16.7632290459637</v>
+        <v>80.69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>335</v>
       </c>
       <c r="B14" t="n">
-        <v>18.5786017767478</v>
+        <v>80.37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>328</v>
       </c>
       <c r="B15" t="n">
-        <v>17.7288528389339</v>
+        <v>79.93</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>287</v>
       </c>
       <c r="B16" t="n">
-        <v>14.1367323290846</v>
+        <v>79.61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>326</v>
       </c>
       <c r="B17" t="n">
-        <v>17.2653534183082</v>
+        <v>79.61</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>298</v>
       </c>
       <c r="B18" t="n">
-        <v>18.8103514870606</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>301</v>
       </c>
       <c r="B19" t="n">
-        <v>16.8404789494013</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>320</v>
       </c>
       <c r="B20" t="n">
-        <v>17.8447276940904</v>
+        <v>79.28</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>303</v>
       </c>
       <c r="B21" t="n">
-        <v>18.2696021629973</v>
+        <v>79.18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>209</v>
       </c>
       <c r="B22" t="n">
-        <v>20.5098493626883</v>
+        <v>79.07</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="B23" t="n">
-        <v>20.2394747006566</v>
+        <v>78.96</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>366</v>
       </c>
       <c r="B24" t="n">
-        <v>17.0722286597142</v>
+        <v>78.74</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>312</v>
       </c>
       <c r="B25" t="n">
-        <v>20.0463499420626</v>
+        <v>78.52</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>274</v>
       </c>
       <c r="B26" t="n">
-        <v>18.4627269215914</v>
+        <v>78.42</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>273</v>
       </c>
       <c r="B27" t="n">
-        <v>18.4241019698725</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>302</v>
       </c>
       <c r="B28" t="n">
-        <v>19.6214754731557</v>
+        <v>78.09</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>323</v>
       </c>
       <c r="B29" t="n">
-        <v>16.1452298184627</v>
+        <v>78.09</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>271</v>
       </c>
       <c r="B30" t="n">
-        <v>17.8833526458092</v>
+        <v>77.98</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>358</v>
       </c>
       <c r="B31" t="n">
-        <v>17.9992275009656</v>
+        <v>77.98</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>283</v>
       </c>
       <c r="B32" t="n">
-        <v>12.3213595983005</v>
+        <v>77.87</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="B33" t="n">
-        <v>19.1966010042487</v>
+        <v>77.77</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>333</v>
       </c>
       <c r="B34" t="n">
-        <v>17.3426033217458</v>
+        <v>77.66</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>352</v>
       </c>
       <c r="B35" t="n">
-        <v>17.0722286597142</v>
+        <v>77.66</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>262</v>
       </c>
       <c r="B36" t="n">
-        <v>16.1066048667439</v>
+        <v>77.55</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>276</v>
       </c>
       <c r="B37" t="n">
-        <v>17.6902278872151</v>
+        <v>77.55</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>289</v>
       </c>
       <c r="B38" t="n">
-        <v>18.1537273078409</v>
+        <v>77.55</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>308</v>
       </c>
       <c r="B39" t="n">
-        <v>18.3082271147161</v>
+        <v>77.55</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>259</v>
       </c>
       <c r="B40" t="n">
-        <v>18.2309772112785</v>
+        <v>77.22</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>294</v>
       </c>
       <c r="B41" t="n">
-        <v>20.0077249903438</v>
+        <v>77.22</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>304</v>
       </c>
       <c r="B42" t="n">
-        <v>19.0807261490923</v>
+        <v>77.11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>334</v>
       </c>
       <c r="B43" t="n">
-        <v>20.162224797219</v>
+        <v>77.11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>306</v>
       </c>
       <c r="B44" t="n">
-        <v>14.5229818462727</v>
+        <v>76.9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>329</v>
       </c>
       <c r="B45" t="n">
-        <v>17.303978370027</v>
+        <v>76.79</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="B46" t="n">
-        <v>19.351100811124</v>
+        <v>76.68</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>293</v>
       </c>
       <c r="B47" t="n">
-        <v>17.2267284665894</v>
+        <v>76.68</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="B48" t="n">
-        <v>12.8621089223638</v>
+        <v>76.57</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>338</v>
       </c>
       <c r="B49" t="n">
-        <v>14.4457319428351</v>
+        <v>76.46</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>349</v>
       </c>
       <c r="B50" t="n">
-        <v>18.1923522595597</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>381</v>
       </c>
       <c r="B51" t="n">
-        <v>16.1066048667439</v>
+        <v>75.7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>292</v>
       </c>
       <c r="B52" t="n">
-        <v>16.3769795287756</v>
+        <v>75.6</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>300</v>
       </c>
       <c r="B53" t="n">
-        <v>12.3599845500193</v>
+        <v>75.6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>305</v>
       </c>
       <c r="B54" t="n">
-        <v>13.441483198146</v>
+        <v>75.6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>337</v>
       </c>
       <c r="B55" t="n">
-        <v>15.3341058323677</v>
+        <v>75.49</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>357</v>
       </c>
       <c r="B56" t="n">
-        <v>14.4457319428351</v>
+        <v>75.38</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>272</v>
       </c>
       <c r="B57" t="n">
-        <v>15.1796060254925</v>
+        <v>75.27</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>288</v>
       </c>
       <c r="B58" t="n">
-        <v>14.4071069911163</v>
+        <v>75.27</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>332</v>
       </c>
       <c r="B59" t="n">
-        <v>14.9092313634608</v>
+        <v>75.27</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>346</v>
       </c>
       <c r="B60" t="n">
-        <v>13.9822325222093</v>
+        <v>75.16</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>286</v>
       </c>
       <c r="B61" t="n">
-        <v>14.4843568945539</v>
+        <v>75.05</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>296</v>
       </c>
       <c r="B62" t="n">
-        <v>13.0166087292391</v>
+        <v>75.05</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>345</v>
       </c>
       <c r="B63" t="n">
-        <v>14.6002317497103</v>
+        <v>75.05</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>200</v>
       </c>
       <c r="B64" t="n">
-        <v>12.4758594051757</v>
+        <v>74.95</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>313</v>
       </c>
       <c r="B65" t="n">
-        <v>13.4801081498648</v>
+        <v>74.95</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>317</v>
       </c>
       <c r="B66" t="n">
-        <v>14.059482425647</v>
+        <v>74.95</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>281</v>
       </c>
       <c r="B67" t="n">
-        <v>14.7161066048667</v>
+        <v>74.84</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>307</v>
       </c>
       <c r="B68" t="n">
-        <v>13.1711085361143</v>
+        <v>74.84</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="B69" t="n">
-        <v>12.2827346465817</v>
+        <v>74.73</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>282</v>
       </c>
       <c r="B70" t="n">
-        <v>13.7118578601777</v>
+        <v>74.73</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>275</v>
       </c>
       <c r="B71" t="n">
-        <v>18.6172267284666</v>
+        <v>74.62</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>344</v>
       </c>
       <c r="B72" t="n">
-        <v>11.5102356122055</v>
+        <v>74.62</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>260</v>
       </c>
       <c r="B73" t="n">
-        <v>13.8663576670529</v>
+        <v>74.4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>330</v>
       </c>
       <c r="B74" t="n">
-        <v>14.870606411742</v>
+        <v>74.4</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="B75" t="n">
-        <v>15.4113557358053</v>
+        <v>74.3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>379</v>
       </c>
       <c r="B76" t="n">
-        <v>14.7547315565856</v>
+        <v>74.3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>336</v>
       </c>
       <c r="B77" t="n">
-        <v>16.492854383932</v>
+        <v>74.19</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>311</v>
       </c>
       <c r="B78" t="n">
-        <v>15.5658555426806</v>
+        <v>73.97</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>347</v>
       </c>
       <c r="B79" t="n">
-        <v>13.4028582464272</v>
+        <v>73.86</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>365</v>
       </c>
       <c r="B80" t="n">
-        <v>12.0509849362688</v>
+        <v>73.86</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>373</v>
       </c>
       <c r="B81" t="n">
-        <v>14.0981073773658</v>
+        <v>73.75</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>170</v>
       </c>
       <c r="B82" t="n">
-        <v>11.7033603707995</v>
+        <v>73.64</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>324</v>
       </c>
       <c r="B83" t="n">
-        <v>15.2954808806489</v>
+        <v>73.54</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>340</v>
       </c>
       <c r="B84" t="n">
-        <v>12.3986095017381</v>
+        <v>73.54</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>375</v>
       </c>
       <c r="B85" t="n">
-        <v>14.9478563151796</v>
+        <v>73.54</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>85</v>
+        <v>165</v>
       </c>
       <c r="B86" t="n">
-        <v>16.492854383932</v>
+        <v>73.21</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>86</v>
+        <v>370</v>
       </c>
       <c r="B87" t="n">
-        <v>14.2912321359598</v>
+        <v>73.21</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>87</v>
+        <v>211</v>
       </c>
       <c r="B88" t="n">
-        <v>14.3684820393975</v>
+        <v>73.1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>88</v>
+        <v>378</v>
       </c>
       <c r="B89" t="n">
-        <v>21.1664735419081</v>
+        <v>73.1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>89</v>
+        <v>343</v>
       </c>
       <c r="B90" t="n">
-        <v>19.5056006179992</v>
+        <v>72.99</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>90</v>
+        <v>364</v>
       </c>
       <c r="B91" t="n">
-        <v>12.5531093086134</v>
+        <v>72.99</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>91</v>
+        <v>269</v>
       </c>
       <c r="B92" t="n">
-        <v>13.8277327153341</v>
+        <v>72.89</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="B93" t="n">
-        <v>13.7118578601777</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>93</v>
+        <v>181</v>
       </c>
       <c r="B94" t="n">
-        <v>12.5917342603322</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="B95" t="n">
-        <v>15.2568559289301</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>279</v>
       </c>
       <c r="B96" t="n">
-        <v>11.8578601776748</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>96</v>
+        <v>280</v>
       </c>
       <c r="B97" t="n">
-        <v>13.248358439552</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>97</v>
+        <v>321</v>
       </c>
       <c r="B98" t="n">
-        <v>18.4241019698725</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>98</v>
+        <v>376</v>
       </c>
       <c r="B99" t="n">
-        <v>14.2139822325222</v>
+        <v>72.78</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>99</v>
+        <v>353</v>
       </c>
       <c r="B100" t="n">
-        <v>16.1838547701815</v>
+        <v>72.67</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>100</v>
+        <v>205</v>
       </c>
       <c r="B101" t="n">
-        <v>15.9521050598687</v>
+        <v>72.56</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>101</v>
+        <v>299</v>
       </c>
       <c r="B102" t="n">
-        <v>16.492854383932</v>
+        <v>72.56</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="B103" t="n">
-        <v>14.0981073773658</v>
+        <v>72.45</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>103</v>
+        <v>193</v>
       </c>
       <c r="B104" t="n">
-        <v>13.5959830050212</v>
+        <v>72.45</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>104</v>
+        <v>266</v>
       </c>
       <c r="B105" t="n">
-        <v>15.6431054461182</v>
+        <v>72.34</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="B106" t="n">
-        <v>12.9779837775203</v>
+        <v>72.23</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="B107" t="n">
-        <v>11.0853611432986</v>
+        <v>72.23</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>107</v>
+        <v>339</v>
       </c>
       <c r="B108" t="n">
-        <v>12.2827346465817</v>
+        <v>72.23</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>108</v>
+        <v>342</v>
       </c>
       <c r="B109" t="n">
-        <v>14.870606411742</v>
+        <v>72.13</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>109</v>
+        <v>362</v>
       </c>
       <c r="B110" t="n">
-        <v>14.9092313634608</v>
+        <v>72.13</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>110</v>
+        <v>284</v>
       </c>
       <c r="B111" t="n">
-        <v>22.1707222865971</v>
+        <v>72.02</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="B112" t="n">
-        <v>12.630359212051</v>
+        <v>72.02</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>112</v>
+        <v>341</v>
       </c>
       <c r="B113" t="n">
-        <v>12.0509849362688</v>
+        <v>71.91</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="B114" t="n">
-        <v>15.3341058323677</v>
+        <v>71.69</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>114</v>
+        <v>318</v>
       </c>
       <c r="B115" t="n">
-        <v>15.6044804943994</v>
+        <v>71.58</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="B116" t="n">
-        <v>15.4113557358053</v>
+        <v>71.48</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>116</v>
+        <v>310</v>
       </c>
       <c r="B117" t="n">
-        <v>15.3341058323677</v>
+        <v>71.37</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>117</v>
+        <v>355</v>
       </c>
       <c r="B118" t="n">
-        <v>11.819235225956</v>
+        <v>71.37</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>118</v>
+        <v>315</v>
       </c>
       <c r="B119" t="n">
-        <v>11.819235225956</v>
+        <v>71.26</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>119</v>
+        <v>360</v>
       </c>
       <c r="B120" t="n">
-        <v>19.351100811124</v>
+        <v>71.26</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>120</v>
+        <v>270</v>
       </c>
       <c r="B121" t="n">
-        <v>11.7806102742372</v>
+        <v>71.15</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="B122" t="n">
-        <v>14.0208574739282</v>
+        <v>71.04</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B123" t="n">
-        <v>16.9563538045577</v>
+        <v>71.04</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>123</v>
+        <v>309</v>
       </c>
       <c r="B124" t="n">
-        <v>16.1838547701815</v>
+        <v>71.04</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>124</v>
+        <v>327</v>
       </c>
       <c r="B125" t="n">
-        <v>13.9822325222093</v>
+        <v>71.04</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>125</v>
+        <v>351</v>
       </c>
       <c r="B126" t="n">
-        <v>15.2954808806489</v>
+        <v>70.93</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>126</v>
+        <v>177</v>
       </c>
       <c r="B127" t="n">
-        <v>14.6002317497103</v>
+        <v>70.82</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>127</v>
+        <v>322</v>
       </c>
       <c r="B128" t="n">
-        <v>14.4457319428351</v>
+        <v>70.72</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>128</v>
+        <v>261</v>
       </c>
       <c r="B129" t="n">
-        <v>14.4457319428351</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="B130" t="n">
-        <v>15.063731170336</v>
+        <v>70.28</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="B131" t="n">
-        <v>15.2182309772113</v>
+        <v>70.28</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>131</v>
+        <v>290</v>
       </c>
       <c r="B132" t="n">
-        <v>18.7717265353418</v>
+        <v>70.28</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="B133" t="n">
-        <v>17.1494785631518</v>
+        <v>70.07</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>133</v>
+        <v>319</v>
       </c>
       <c r="B134" t="n">
-        <v>17.3426033217458</v>
+        <v>70.07</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="B135" t="n">
-        <v>15.3727307840865</v>
+        <v>69.85</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>135</v>
+        <v>348</v>
       </c>
       <c r="B136" t="n">
-        <v>13.9049826187717</v>
+        <v>69.85</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>136</v>
+        <v>79</v>
       </c>
       <c r="B137" t="n">
-        <v>17.921977597528</v>
+        <v>69.74</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="B138" t="n">
-        <v>14.7933565083044</v>
+        <v>69.74</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="B139" t="n">
-        <v>15.681730397837</v>
+        <v>69.63</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>139</v>
+        <v>295</v>
       </c>
       <c r="B140" t="n">
-        <v>12.1282348397065</v>
+        <v>69.41</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="B141" t="n">
-        <v>18.1537273078409</v>
+        <v>69.2</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B142" t="n">
-        <v>15.2954808806489</v>
+        <v>69.09</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="B143" t="n">
-        <v>16.0679799150251</v>
+        <v>68.98</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="B144" t="n">
-        <v>14.7933565083044</v>
+        <v>68.98</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>144</v>
+        <v>255</v>
       </c>
       <c r="B145" t="n">
-        <v>12.5531093086134</v>
+        <v>68.98</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>145</v>
+        <v>264</v>
       </c>
       <c r="B146" t="n">
-        <v>14.7547315565856</v>
+        <v>68.98</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="B147" t="n">
-        <v>14.2139822325222</v>
+        <v>68.66</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>147</v>
+        <v>350</v>
       </c>
       <c r="B148" t="n">
-        <v>14.870606411742</v>
+        <v>68.66</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>148</v>
+        <v>47</v>
       </c>
       <c r="B149" t="n">
-        <v>13.5959830050212</v>
+        <v>68.44</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="B150" t="n">
-        <v>15.8748551564311</v>
+        <v>68.33</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>150</v>
+        <v>291</v>
       </c>
       <c r="B151" t="n">
-        <v>16.0293549633063</v>
+        <v>68.33</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B152" t="n">
-        <v>14.252607184241</v>
+        <v>68.22</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>152</v>
+        <v>265</v>
       </c>
       <c r="B153" t="n">
-        <v>15.9134801081499</v>
+        <v>68.22</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="B154" t="n">
-        <v>8.61336423329471</v>
+        <v>68.11</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B155" t="n">
-        <v>10.0424874468907</v>
+        <v>68.11</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>155</v>
+        <v>367</v>
       </c>
       <c r="B156" t="n">
-        <v>13.8277327153341</v>
+        <v>68.11</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>156</v>
+        <v>314</v>
       </c>
       <c r="B157" t="n">
-        <v>13.6346079567401</v>
+        <v>68</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>157</v>
+        <v>354</v>
       </c>
       <c r="B158" t="n">
-        <v>9.11548860563924</v>
+        <v>68</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>158</v>
+        <v>356</v>
       </c>
       <c r="B159" t="n">
-        <v>12.5144843568946</v>
+        <v>68</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>159</v>
+        <v>359</v>
       </c>
       <c r="B160" t="n">
-        <v>11.6647354190807</v>
+        <v>68</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>160</v>
+        <v>297</v>
       </c>
       <c r="B161" t="n">
-        <v>6.52761684047895</v>
+        <v>67.9</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>161</v>
+        <v>316</v>
       </c>
       <c r="B162" t="n">
-        <v>8.80648899188876</v>
+        <v>67.9</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="B163" t="n">
-        <v>5.79374275782155</v>
+        <v>67.79</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="B164" t="n">
-        <v>10.1969872537659</v>
+        <v>67.79</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="B165" t="n">
-        <v>15.2954808806489</v>
+        <v>67.79</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="B166" t="n">
-        <v>10.1583623020471</v>
+        <v>67.46</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="B167" t="n">
-        <v>6.48899188876014</v>
+        <v>67.35</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="B168" t="n">
-        <v>13.6732329084589</v>
+        <v>67.25</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>12.01235998455</v>
+        <v>67.25</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="B170" t="n">
-        <v>10.8536114329857</v>
+        <v>67.25</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="B171" t="n">
-        <v>9.81073773657783</v>
+        <v>67.14</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B172" t="n">
-        <v>14.2139822325222</v>
+        <v>67.03</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="B173" t="n">
-        <v>11.8964851293936</v>
+        <v>66.92</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="B174" t="n">
-        <v>11.5102356122055</v>
+        <v>66.81</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>174</v>
+        <v>380</v>
       </c>
       <c r="B175" t="n">
-        <v>14.7547315565856</v>
+        <v>66.81</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B176" t="n">
-        <v>15.1023561220548</v>
+        <v>66.7</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>176</v>
+        <v>63</v>
       </c>
       <c r="B177" t="n">
-        <v>12.0509849362688</v>
+        <v>66.49</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="B178" t="n">
-        <v>11.8964851293936</v>
+        <v>66.49</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="B179" t="n">
-        <v>14.059482425647</v>
+        <v>66.49</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B180" t="n">
-        <v>13.3642332947084</v>
+        <v>66.49</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="B181" t="n">
-        <v>13.3642332947084</v>
+        <v>66.38</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B182" t="n">
-        <v>11.6261104673619</v>
+        <v>66.38</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="B183" t="n">
-        <v>11.819235225956</v>
+        <v>66.27</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>183</v>
+        <v>371</v>
       </c>
       <c r="B184" t="n">
-        <v>14.4071069911163</v>
+        <v>66.16</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B185" t="n">
-        <v>12.8621089223638</v>
+        <v>65.84</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>185</v>
+        <v>83</v>
       </c>
       <c r="B186" t="n">
-        <v>11.0853611432986</v>
+        <v>65.73</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="B187" t="n">
-        <v>16.1452298184627</v>
+        <v>65.73</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B188" t="n">
-        <v>13.1711085361143</v>
+        <v>65.73</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>188</v>
+        <v>256</v>
       </c>
       <c r="B189" t="n">
-        <v>13.4801081498648</v>
+        <v>65.73</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>189</v>
+        <v>374</v>
       </c>
       <c r="B190" t="n">
-        <v>14.0981073773658</v>
+        <v>65.62</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>190</v>
+        <v>67</v>
       </c>
       <c r="B191" t="n">
-        <v>10.9694862881421</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>191</v>
+        <v>78</v>
       </c>
       <c r="B192" t="n">
-        <v>14.9478563151796</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>192</v>
+        <v>90</v>
       </c>
       <c r="B193" t="n">
-        <v>11.008111239861</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B194" t="n">
-        <v>11.5102356122055</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>194</v>
+        <v>250</v>
       </c>
       <c r="B195" t="n">
-        <v>16.1452298184627</v>
+        <v>65.51</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="B196" t="n">
-        <v>13.2869833912708</v>
+        <v>65.29</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B197" t="n">
-        <v>10.39011201236</v>
+        <v>65.29</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="B198" t="n">
-        <v>9.38586326767092</v>
+        <v>65.29</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="B199" t="n">
-        <v>13.4028582464272</v>
+        <v>65.18</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>199</v>
+        <v>253</v>
       </c>
       <c r="B200" t="n">
-        <v>15.7976052529934</v>
+        <v>65.18</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="B201" t="n">
-        <v>10.0424874468907</v>
+        <v>65.08</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>201</v>
+        <v>372</v>
       </c>
       <c r="B202" t="n">
-        <v>15.9907300115875</v>
+        <v>65.08</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="B203" t="n">
-        <v>12.0896098879876</v>
+        <v>64.97</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="B204" t="n">
-        <v>13.9822325222093</v>
+        <v>64.97</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>204</v>
+        <v>111</v>
       </c>
       <c r="B205" t="n">
-        <v>17.4198532251835</v>
+        <v>64.86</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>205</v>
+        <v>64</v>
       </c>
       <c r="B206" t="n">
-        <v>11.6261104673619</v>
+        <v>64.64</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="B207" t="n">
-        <v>14.0981073773658</v>
+        <v>64.53</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>207</v>
+        <v>246</v>
       </c>
       <c r="B208" t="n">
-        <v>14.6388567014291</v>
+        <v>64.43</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>208</v>
+        <v>80</v>
       </c>
       <c r="B209" t="n">
-        <v>7.49324063344921</v>
+        <v>64.32</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>209</v>
+        <v>105</v>
       </c>
       <c r="B210" t="n">
-        <v>9.19273850907686</v>
+        <v>64.32</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="B211" t="n">
-        <v>10.8536114329857</v>
+        <v>64.32</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="B212" t="n">
-        <v>10.8149864812669</v>
+        <v>63.99</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>212</v>
+        <v>72</v>
       </c>
       <c r="B213" t="n">
-        <v>18.5013518733102</v>
+        <v>63.88</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>213</v>
+        <v>60</v>
       </c>
       <c r="B214" t="n">
-        <v>17.3426033217458</v>
+        <v>63.77</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>214</v>
+        <v>53</v>
       </c>
       <c r="B215" t="n">
-        <v>15.2568559289301</v>
+        <v>63.56</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>215</v>
+        <v>96</v>
       </c>
       <c r="B216" t="n">
-        <v>15.8362302047122</v>
+        <v>63.56</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>216</v>
+        <v>73</v>
       </c>
       <c r="B217" t="n">
-        <v>16.6859791425261</v>
+        <v>63.34</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>217</v>
+        <v>164</v>
       </c>
       <c r="B218" t="n">
-        <v>16.8018539976825</v>
+        <v>63.34</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>218</v>
+        <v>368</v>
       </c>
       <c r="B219" t="n">
-        <v>15.681730397837</v>
+        <v>63.34</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>219</v>
+        <v>361</v>
       </c>
       <c r="B220" t="n">
-        <v>17.0722286597142</v>
+        <v>63.23</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>220</v>
+        <v>74</v>
       </c>
       <c r="B221" t="n">
-        <v>16.3769795287756</v>
+        <v>63.02</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>221</v>
+        <v>175</v>
       </c>
       <c r="B222" t="n">
-        <v>16.492854383932</v>
+        <v>62.91</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>222</v>
+        <v>48</v>
       </c>
       <c r="B223" t="n">
-        <v>16.7632290459637</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>223</v>
+        <v>75</v>
       </c>
       <c r="B224" t="n">
-        <v>21.6685979142526</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="B225" t="n">
-        <v>15.5272305909618</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>225</v>
+        <v>77</v>
       </c>
       <c r="B226" t="n">
-        <v>18.9648512939359</v>
+        <v>62.58</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>226</v>
+        <v>103</v>
       </c>
       <c r="B227" t="n">
-        <v>19.4283507145616</v>
+        <v>62.58</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="B228" t="n">
-        <v>15.7589803012746</v>
+        <v>62.58</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B229" t="n">
-        <v>19.351100811124</v>
+        <v>62.58</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>229</v>
+        <v>148</v>
       </c>
       <c r="B230" t="n">
-        <v>18.0764774044032</v>
+        <v>62.47</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>230</v>
+        <v>69</v>
       </c>
       <c r="B231" t="n">
-        <v>15.681730397837</v>
+        <v>62.26</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>231</v>
+        <v>135</v>
       </c>
       <c r="B232" t="n">
-        <v>16.8018539976825</v>
+        <v>62.04</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="B233" t="n">
-        <v>12.3599845500193</v>
+        <v>62.04</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>233</v>
+        <v>15</v>
       </c>
       <c r="B234" t="n">
-        <v>14.8319814600232</v>
+        <v>61.93</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>234</v>
+        <v>92</v>
       </c>
       <c r="B235" t="n">
-        <v>13.4801081498648</v>
+        <v>61.93</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>235</v>
+        <v>57</v>
       </c>
       <c r="B236" t="n">
-        <v>19.7373503283121</v>
+        <v>61.71</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>236</v>
+        <v>91</v>
       </c>
       <c r="B237" t="n">
-        <v>12.9007338740827</v>
+        <v>61.71</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>237</v>
+        <v>65</v>
       </c>
       <c r="B238" t="n">
-        <v>14.059482425647</v>
+        <v>61.61</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>238</v>
+        <v>142</v>
       </c>
       <c r="B239" t="n">
-        <v>15.4499806875241</v>
+        <v>61.39</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B240" t="n">
-        <v>15.2954808806489</v>
+        <v>61.39</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="B241" t="n">
-        <v>13.7118578601777</v>
+        <v>61.39</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>241</v>
+        <v>121</v>
       </c>
       <c r="B242" t="n">
-        <v>15.8362302047122</v>
+        <v>61.28</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>242</v>
+        <v>124</v>
       </c>
       <c r="B243" t="n">
-        <v>16.492854383932</v>
+        <v>61.28</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>243</v>
+        <v>186</v>
       </c>
       <c r="B244" t="n">
-        <v>16.1452298184627</v>
+        <v>61.28</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>244</v>
+        <v>2</v>
       </c>
       <c r="B245" t="n">
-        <v>15.5272305909618</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>245</v>
+        <v>55</v>
       </c>
       <c r="B246" t="n">
-        <v>15.1409810737737</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>246</v>
+        <v>62</v>
       </c>
       <c r="B247" t="n">
-        <v>13.4028582464272</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>247</v>
+        <v>86</v>
       </c>
       <c r="B248" t="n">
-        <v>15.6431054461182</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>248</v>
+        <v>102</v>
       </c>
       <c r="B249" t="n">
-        <v>16.1838547701815</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>249</v>
+        <v>87</v>
       </c>
       <c r="B250" t="n">
-        <v>14.0981073773658</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>250</v>
+        <v>146</v>
       </c>
       <c r="B251" t="n">
-        <v>13.1711085361143</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>251</v>
+        <v>151</v>
       </c>
       <c r="B252" t="n">
-        <v>16.6473541908073</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="B253" t="n">
-        <v>12.7462340672074</v>
+        <v>60.95</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="B254" t="n">
-        <v>13.7504828118965</v>
+        <v>60.85</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>254</v>
+        <v>58</v>
       </c>
       <c r="B255" t="n">
-        <v>16.8791039011201</v>
+        <v>60.74</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>255</v>
+        <v>98</v>
       </c>
       <c r="B256" t="n">
-        <v>12.0509849362688</v>
+        <v>60.74</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>256</v>
+        <v>66</v>
       </c>
       <c r="B257" t="n">
-        <v>13.2869833912708</v>
+        <v>60.63</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B258" t="n">
-        <v>14.2139822325222</v>
+        <v>60.63</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>258</v>
+        <v>43</v>
       </c>
       <c r="B259" t="n">
-        <v>10.0811123986095</v>
+        <v>60.52</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>259</v>
+        <v>201</v>
       </c>
       <c r="B260" t="n">
-        <v>8.22711471610661</v>
+        <v>60.52</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>260</v>
+        <v>127</v>
       </c>
       <c r="B261" t="n">
-        <v>9.3086133642333</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="B262" t="n">
-        <v>11.1626110467362</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>262</v>
+        <v>50</v>
       </c>
       <c r="B263" t="n">
-        <v>8.03398995751255</v>
+        <v>59.98</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>263</v>
+        <v>214</v>
       </c>
       <c r="B264" t="n">
-        <v>10.8922363847045</v>
+        <v>59.87</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B265" t="n">
-        <v>11.3557358053302</v>
+        <v>59.87</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>265</v>
+        <v>54</v>
       </c>
       <c r="B266" t="n">
-        <v>11.6647354190807</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>266</v>
+        <v>56</v>
       </c>
       <c r="B267" t="n">
-        <v>10.0424874468907</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>267</v>
+        <v>82</v>
       </c>
       <c r="B268" t="n">
-        <v>6.60486674391657</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>268</v>
+        <v>94</v>
       </c>
       <c r="B269" t="n">
-        <v>6.21861722672847</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>269</v>
+        <v>128</v>
       </c>
       <c r="B270" t="n">
-        <v>9.77211278485902</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="B271" t="n">
-        <v>10.6218617226728</v>
+        <v>59.65</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="B272" t="n">
-        <v>7.87949015063731</v>
+        <v>59.54</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>272</v>
+        <v>126</v>
       </c>
       <c r="B273" t="n">
-        <v>8.88373889532638</v>
+        <v>59.44</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="B274" t="n">
-        <v>7.95674005407493</v>
+        <v>59.33</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>274</v>
+        <v>145</v>
       </c>
       <c r="B275" t="n">
-        <v>7.72499034376207</v>
+        <v>59.22</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>275</v>
+        <v>108</v>
       </c>
       <c r="B276" t="n">
-        <v>9.15411355735805</v>
+        <v>59.11</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>276</v>
+        <v>147</v>
       </c>
       <c r="B277" t="n">
-        <v>8.18848976438779</v>
+        <v>59.11</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="B278" t="n">
-        <v>9.19273850907686</v>
+        <v>59</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>278</v>
+        <v>84</v>
       </c>
       <c r="B279" t="n">
-        <v>5.33024333719583</v>
+        <v>58.89</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>279</v>
+        <v>137</v>
       </c>
       <c r="B280" t="n">
-        <v>9.84936268829664</v>
+        <v>58.89</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="B281" t="n">
-        <v>9.88798764001545</v>
+        <v>58.89</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="B282" t="n">
-        <v>9.03823870220162</v>
+        <v>58.79</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>282</v>
+        <v>224</v>
       </c>
       <c r="B283" t="n">
-        <v>9.03823870220162</v>
+        <v>58.68</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>283</v>
+        <v>109</v>
       </c>
       <c r="B284" t="n">
-        <v>7.91811510235612</v>
+        <v>58.57</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>284</v>
+        <v>143</v>
       </c>
       <c r="B285" t="n">
-        <v>10.1197373503283</v>
+        <v>58.57</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>285</v>
+        <v>125</v>
       </c>
       <c r="B286" t="n">
-        <v>8.38161452298185</v>
+        <v>58.46</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>286</v>
+        <v>227</v>
       </c>
       <c r="B287" t="n">
-        <v>9.03823870220162</v>
+        <v>58.35</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>287</v>
+        <v>113</v>
       </c>
       <c r="B288" t="n">
-        <v>7.41599073001159</v>
+        <v>58.24</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="B289" t="n">
-        <v>8.99961375048281</v>
+        <v>58.24</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>289</v>
+        <v>218</v>
       </c>
       <c r="B290" t="n">
-        <v>8.11123986095017</v>
+        <v>58.13</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>290</v>
+        <v>243</v>
       </c>
       <c r="B291" t="n">
-        <v>10.8536114329857</v>
+        <v>58.13</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>291</v>
+        <v>129</v>
       </c>
       <c r="B292" t="n">
-        <v>11.6261104673619</v>
+        <v>58.03</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>292</v>
+        <v>130</v>
       </c>
       <c r="B293" t="n">
-        <v>8.76786404016995</v>
+        <v>58.03</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>293</v>
+        <v>115</v>
       </c>
       <c r="B294" t="n">
-        <v>8.80648899188876</v>
+        <v>57.92</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>294</v>
+        <v>76</v>
       </c>
       <c r="B295" t="n">
-        <v>8.30436461954423</v>
+        <v>57.81</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>295</v>
+        <v>219</v>
       </c>
       <c r="B296" t="n">
-        <v>11.7419853225183</v>
+        <v>57.81</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>296</v>
+        <v>51</v>
       </c>
       <c r="B297" t="n">
-        <v>8.92236384704519</v>
+        <v>57.7</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>297</v>
+        <v>134</v>
       </c>
       <c r="B298" t="n">
-        <v>11.5874855156431</v>
+        <v>57.7</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>298</v>
+        <v>116</v>
       </c>
       <c r="B299" t="n">
-        <v>7.76361529548088</v>
+        <v>57.59</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>299</v>
+        <v>215</v>
       </c>
       <c r="B300" t="n">
-        <v>10.0424874468907</v>
+        <v>57.59</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>300</v>
+        <v>141</v>
       </c>
       <c r="B301" t="n">
-        <v>8.72923908845114</v>
+        <v>57.48</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>301</v>
+        <v>242</v>
       </c>
       <c r="B302" t="n">
-        <v>7.4546156817304</v>
+        <v>57.48</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>302</v>
+        <v>221</v>
       </c>
       <c r="B303" t="n">
-        <v>7.91811510235612</v>
+        <v>57.38</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>303</v>
+        <v>241</v>
       </c>
       <c r="B304" t="n">
-        <v>7.57049053688683</v>
+        <v>57.38</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>304</v>
+        <v>216</v>
       </c>
       <c r="B305" t="n">
-        <v>8.18848976438779</v>
+        <v>57.27</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>305</v>
+        <v>150</v>
       </c>
       <c r="B306" t="n">
-        <v>8.80648899188876</v>
+        <v>57.16</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>306</v>
+        <v>217</v>
       </c>
       <c r="B307" t="n">
-        <v>8.30436461954423</v>
+        <v>57.16</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>307</v>
+        <v>220</v>
       </c>
       <c r="B308" t="n">
-        <v>9.03823870220162</v>
+        <v>57.05</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>308</v>
+        <v>138</v>
       </c>
       <c r="B309" t="n">
-        <v>8.11123986095017</v>
+        <v>56.94</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>309</v>
+        <v>213</v>
       </c>
       <c r="B310" t="n">
-        <v>11.0467361915798</v>
+        <v>56.94</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>310</v>
+        <v>85</v>
       </c>
       <c r="B311" t="n">
-        <v>10.583236770954</v>
+        <v>56.83</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>311</v>
+        <v>123</v>
       </c>
       <c r="B312" t="n">
-        <v>9.57898802626497</v>
+        <v>56.83</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>312</v>
+        <v>152</v>
       </c>
       <c r="B313" t="n">
-        <v>7.68636539204326</v>
+        <v>56.83</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>313</v>
+        <v>9</v>
       </c>
       <c r="B314" t="n">
-        <v>9.19273850907686</v>
+        <v>56.72</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>314</v>
+        <v>28</v>
       </c>
       <c r="B315" t="n">
-        <v>11.7033603707995</v>
+        <v>56.62</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>315</v>
+        <v>35</v>
       </c>
       <c r="B316" t="n">
-        <v>10.8922363847045</v>
+        <v>56.62</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>316</v>
+        <v>104</v>
       </c>
       <c r="B317" t="n">
-        <v>12.2827346465817</v>
+        <v>56.51</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>317</v>
+        <v>114</v>
       </c>
       <c r="B318" t="n">
-        <v>8.99961375048281</v>
+        <v>56.51</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>318</v>
+        <v>100</v>
       </c>
       <c r="B319" t="n">
-        <v>10.1969872537659</v>
+        <v>56.29</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>319</v>
+        <v>149</v>
       </c>
       <c r="B320" t="n">
-        <v>11.008111239861</v>
+        <v>56.18</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>320</v>
+        <v>231</v>
       </c>
       <c r="B321" t="n">
-        <v>7.4546156817304</v>
+        <v>56.07</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>321</v>
+        <v>11</v>
       </c>
       <c r="B322" t="n">
-        <v>9.81073773657783</v>
+        <v>55.97</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>322</v>
+        <v>49</v>
       </c>
       <c r="B323" t="n">
-        <v>10.6991116261105</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>323</v>
+        <v>70</v>
       </c>
       <c r="B324" t="n">
-        <v>7.95674005407493</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>324</v>
+        <v>122</v>
       </c>
       <c r="B325" t="n">
-        <v>9.6948628814214</v>
+        <v>55.42</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>325</v>
+        <v>99</v>
       </c>
       <c r="B326" t="n">
-        <v>5.87099266125917</v>
+        <v>55.31</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>326</v>
+        <v>101</v>
       </c>
       <c r="B327" t="n">
-        <v>7.33874082657397</v>
+        <v>54.66</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>327</v>
+        <v>18</v>
       </c>
       <c r="B328" t="n">
-        <v>10.3514870606412</v>
+        <v>54.34</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>328</v>
+        <v>229</v>
       </c>
       <c r="B329" t="n">
-        <v>7.33874082657397</v>
+        <v>54.12</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>329</v>
+        <v>44</v>
       </c>
       <c r="B330" t="n">
-        <v>8.34298957126304</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>330</v>
+        <v>12</v>
       </c>
       <c r="B331" t="n">
-        <v>9.26998841251448</v>
+        <v>53.69</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>331</v>
+        <v>23</v>
       </c>
       <c r="B332" t="n">
-        <v>10.1969872537659</v>
+        <v>53.69</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>332</v>
+        <v>34</v>
       </c>
       <c r="B333" t="n">
-        <v>8.88373889532638</v>
+        <v>53.69</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>333</v>
+        <v>212</v>
       </c>
       <c r="B334" t="n">
-        <v>7.99536500579374</v>
+        <v>53.47</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>334</v>
+        <v>225</v>
       </c>
       <c r="B335" t="n">
-        <v>8.22711471610661</v>
+        <v>53.47</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>335</v>
+        <v>29</v>
       </c>
       <c r="B336" t="n">
-        <v>7.02974121282348</v>
+        <v>53.15</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>336</v>
+        <v>5</v>
       </c>
       <c r="B337" t="n">
-        <v>9.38586326767092</v>
+        <v>53.04</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>337</v>
+        <v>133</v>
       </c>
       <c r="B338" t="n">
-        <v>8.84511394360757</v>
+        <v>53.04</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>338</v>
+        <v>46</v>
       </c>
       <c r="B339" t="n">
-        <v>8.45886442641947</v>
+        <v>52.93</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>339</v>
+        <v>136</v>
       </c>
       <c r="B340" t="n">
-        <v>10.5059868675164</v>
+        <v>52.82</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>340</v>
+        <v>228</v>
       </c>
       <c r="B341" t="n">
-        <v>9.61761297798378</v>
+        <v>52.82</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>341</v>
+        <v>33</v>
       </c>
       <c r="B342" t="n">
-        <v>10.1197373503283</v>
+        <v>52.6</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>342</v>
+        <v>132</v>
       </c>
       <c r="B343" t="n">
-        <v>10.39011201236</v>
+        <v>52.49</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>343</v>
+        <v>13</v>
       </c>
       <c r="B344" t="n">
-        <v>9.73348783314021</v>
+        <v>52.39</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>344</v>
+        <v>226</v>
       </c>
       <c r="B345" t="n">
-        <v>9.11548860563924</v>
+        <v>52.39</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>345</v>
+        <v>16</v>
       </c>
       <c r="B346" t="n">
-        <v>8.92236384704519</v>
+        <v>52.28</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>346</v>
+        <v>19</v>
       </c>
       <c r="B347" t="n">
-        <v>9.03823870220162</v>
+        <v>52.28</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>347</v>
+        <v>140</v>
       </c>
       <c r="B348" t="n">
-        <v>9.57898802626497</v>
+        <v>52.28</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>348</v>
+        <v>36</v>
       </c>
       <c r="B349" t="n">
-        <v>11.0853611432986</v>
+        <v>51.95</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>349</v>
+        <v>30</v>
       </c>
       <c r="B350" t="n">
-        <v>8.69061413673233</v>
+        <v>51.84</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>350</v>
+        <v>1</v>
       </c>
       <c r="B351" t="n">
-        <v>12.3599845500193</v>
+        <v>51.74</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>351</v>
+        <v>14</v>
       </c>
       <c r="B352" t="n">
-        <v>10.6218617226728</v>
+        <v>51.63</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>352</v>
+        <v>20</v>
       </c>
       <c r="B353" t="n">
-        <v>7.99536500579374</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>353</v>
+        <v>38</v>
       </c>
       <c r="B354" t="n">
-        <v>10.3128621089224</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>354</v>
+        <v>17</v>
       </c>
       <c r="B355" t="n">
-        <v>12.9779837775203</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>355</v>
+        <v>3</v>
       </c>
       <c r="B356" t="n">
-        <v>10.39011201236</v>
+        <v>51.19</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>356</v>
+        <v>37</v>
       </c>
       <c r="B357" t="n">
-        <v>12.9779837775203</v>
+        <v>51.19</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>357</v>
+        <v>235</v>
       </c>
       <c r="B358" t="n">
-        <v>10.2742371572036</v>
+        <v>51.19</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>358</v>
+        <v>131</v>
       </c>
       <c r="B359" t="n">
-        <v>8.11123986095017</v>
+        <v>50.87</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>359</v>
+        <v>25</v>
       </c>
       <c r="B360" t="n">
-        <v>12.4758594051757</v>
+        <v>50.76</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>360</v>
+        <v>39</v>
       </c>
       <c r="B361" t="n">
-        <v>11.1239860950174</v>
+        <v>50.54</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>361</v>
+        <v>97</v>
       </c>
       <c r="B362" t="n">
-        <v>14.2912321359598</v>
+        <v>50.43</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>362</v>
+        <v>26</v>
       </c>
       <c r="B363" t="n">
-        <v>10.4673619157976</v>
+        <v>50.33</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>363</v>
+        <v>45</v>
       </c>
       <c r="B364" t="n">
-        <v>7.64774044032445</v>
+        <v>50.22</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>364</v>
+        <v>8</v>
       </c>
       <c r="B365" t="n">
-        <v>10.6218617226728</v>
+        <v>49.78</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>365</v>
+        <v>223</v>
       </c>
       <c r="B366" t="n">
-        <v>12.5917342603322</v>
+        <v>49.78</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>366</v>
+        <v>119</v>
       </c>
       <c r="B367" t="n">
-        <v>7.60911548860564</v>
+        <v>49.46</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>367</v>
+        <v>10</v>
       </c>
       <c r="B368" t="n">
-        <v>11.7806102742372</v>
+        <v>49.24</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>368</v>
+        <v>32</v>
       </c>
       <c r="B369" t="n">
-        <v>13.8663576670529</v>
+        <v>48.92</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>369</v>
+        <v>41</v>
       </c>
       <c r="B370" t="n">
-        <v>2.39474700656624</v>
+        <v>48.92</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>370</v>
+        <v>89</v>
       </c>
       <c r="B371" t="n">
-        <v>9.92661259173426</v>
+        <v>48.7</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>371</v>
+        <v>27</v>
       </c>
       <c r="B372" t="n">
-        <v>13.5573580533024</v>
+        <v>48.05</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>372</v>
+        <v>40</v>
       </c>
       <c r="B373" t="n">
-        <v>13.0938586326767</v>
+        <v>47.83</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>373</v>
+        <v>7</v>
       </c>
       <c r="B374" t="n">
-        <v>9.88798764001545</v>
+        <v>47.72</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>374</v>
+        <v>24</v>
       </c>
       <c r="B375" t="n">
-        <v>13.7118578601777</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>375</v>
+        <v>21</v>
       </c>
       <c r="B376" t="n">
-        <v>9.65623792970259</v>
+        <v>46.96</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>376</v>
+        <v>110</v>
       </c>
       <c r="B377" t="n">
-        <v>10.2356122054847</v>
+        <v>46.75</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>377</v>
+        <v>22</v>
       </c>
       <c r="B378" t="n">
-        <v>7.80224024719969</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>378</v>
+        <v>88</v>
       </c>
       <c r="B379" t="n">
-        <v>10.5059868675164</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>379</v>
+        <v>42</v>
       </c>
       <c r="B380" t="n">
-        <v>9.96523754345307</v>
+        <v>46.1</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>380</v>
+        <v>6</v>
       </c>
       <c r="B381" t="n">
-        <v>15.5658555426806</v>
+        <v>45.88</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>381</v>
+        <v>4</v>
       </c>
       <c r="B382" t="n">
-        <v>9.3086133642333</v>
+        <v>45.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>